<commit_message>
PullRequest: 179 bug fix
Merge branch fix/dev-4.2.0-bugs-xyh-0829 of git@gitlab.alipay-inc.com:oceanbase/oceanbase-developer-center.git into dev-4.2.0
https://code.alipay.com/oceanbase/oceanbase-developer-center/pull_requests/179?tab=commit

Signed-off-by: 晓康 <xxk268858@oceanbase.com>


* fix(100965540)

* fix(100965540): text change

* chore: user and datasource template replacement
</commit_message>
<xml_diff>
--- a/public/template/en-us/datasource_template.xlsx
+++ b/public/template/en-us/datasource_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoda/Documents/batch import template/datasource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoda/Downloads/批量导入模板文件/datasource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBC8C2-6D8A-4441-8AE4-55AAF8665B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B525B295-9B6A-9B43-92A6-27BCE956FA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33120" windowHeight="20480" xr2:uid="{18472E68-B775-9944-86EC-D9EC4E7A8A18}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -85,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,13 +99,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="4"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -140,17 +132,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -470,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC6230F-C2F4-BB44-A6AC-2B51BADF01D0}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="11" width="20.83203125" style="4" customWidth="1"/>
+    <col min="1" max="11" width="20.83203125" style="3" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -516,58 +505,6 @@
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>